<commit_message>
Minor updates on test simulation
</commit_message>
<xml_diff>
--- a/Prototypes/Plantain/Observed.xlsx
+++ b/Prototypes/Plantain/Observed.xlsx
@@ -845,10 +845,10 @@
   <dimension ref="A1:AI1519"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F1478" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F209" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1487" sqref="A1487"/>
+      <selection pane="bottomRight" activeCell="K209" sqref="K209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9772,10 +9772,10 @@
         <v>61</v>
       </c>
       <c r="H210">
-        <v>62.625</v>
+        <v>462.625</v>
       </c>
       <c r="I210">
-        <v>6.2625000000000002</v>
+        <v>46.262500000000003</v>
       </c>
       <c r="U210">
         <v>26.400732040405273</v>
@@ -9822,10 +9822,10 @@
         <v>61</v>
       </c>
       <c r="H211">
-        <v>124.25</v>
+        <v>524.25</v>
       </c>
       <c r="I211">
-        <v>12.425000000000001</v>
+        <v>52.424999999999997</v>
       </c>
       <c r="U211">
         <v>23.148944854736328</v>
@@ -9872,10 +9872,10 @@
         <v>61</v>
       </c>
       <c r="H212">
-        <v>248.5</v>
+        <v>648.5</v>
       </c>
       <c r="I212">
-        <v>24.85</v>
+        <v>64.849999999999994</v>
       </c>
       <c r="U212">
         <v>21.873819351196289</v>
@@ -9922,10 +9922,10 @@
         <v>61</v>
       </c>
       <c r="H213">
-        <v>324.875</v>
+        <v>724.875</v>
       </c>
       <c r="I213">
-        <v>32.487499999999997</v>
+        <v>72.487499999999997</v>
       </c>
       <c r="U213">
         <v>20.650505065917969</v>
@@ -9972,10 +9972,10 @@
         <v>61</v>
       </c>
       <c r="H214">
-        <v>177.75</v>
+        <v>577.75</v>
       </c>
       <c r="I214">
-        <v>17.774999999999999</v>
+        <v>57.774999999999999</v>
       </c>
       <c r="U214">
         <v>23.796581268310547</v>
@@ -10022,10 +10022,10 @@
         <v>61</v>
       </c>
       <c r="H215">
-        <v>146.875</v>
+        <v>546.875</v>
       </c>
       <c r="I215">
-        <v>14.6875</v>
+        <v>54.6875</v>
       </c>
       <c r="U215">
         <v>23.547220230102539</v>
@@ -10072,10 +10072,10 @@
         <v>61</v>
       </c>
       <c r="H216">
-        <v>226.5</v>
+        <v>626.5</v>
       </c>
       <c r="I216">
-        <v>22.65</v>
+        <v>62.65</v>
       </c>
       <c r="U216">
         <v>20.135255813598633</v>
@@ -10122,10 +10122,10 @@
         <v>61</v>
       </c>
       <c r="H217">
-        <v>174.375</v>
+        <v>574.375</v>
       </c>
       <c r="I217">
-        <v>17.4375</v>
+        <v>57.4375</v>
       </c>
       <c r="U217">
         <v>22.550617218017578</v>
@@ -10172,10 +10172,10 @@
         <v>61</v>
       </c>
       <c r="H218">
-        <v>209.875</v>
+        <v>609.875</v>
       </c>
       <c r="I218">
-        <v>20.987500000000001</v>
+        <v>60.987499999999997</v>
       </c>
       <c r="U218">
         <v>21.414056777954102</v>
@@ -10222,10 +10222,10 @@
         <v>61</v>
       </c>
       <c r="H219">
-        <v>136.5</v>
+        <v>536.5</v>
       </c>
       <c r="I219">
-        <v>13.65</v>
+        <v>53.65</v>
       </c>
       <c r="U219">
         <v>21.342010498046875</v>
@@ -10272,10 +10272,10 @@
         <v>61</v>
       </c>
       <c r="H220">
-        <v>233</v>
+        <v>633</v>
       </c>
       <c r="I220">
-        <v>23.3</v>
+        <v>63.3</v>
       </c>
       <c r="U220">
         <v>22.295782089233398</v>
@@ -10322,10 +10322,10 @@
         <v>61</v>
       </c>
       <c r="H221">
-        <v>173</v>
+        <v>573</v>
       </c>
       <c r="I221">
-        <v>17.3</v>
+        <v>57.3</v>
       </c>
       <c r="U221">
         <v>22.901821136474609</v>
@@ -10372,10 +10372,10 @@
         <v>61</v>
       </c>
       <c r="H222">
-        <v>278.375</v>
+        <v>678.375</v>
       </c>
       <c r="I222">
-        <v>27.837499999999999</v>
+        <v>67.837500000000006</v>
       </c>
       <c r="U222">
         <v>20.649356842041016</v>
@@ -10422,10 +10422,10 @@
         <v>61</v>
       </c>
       <c r="H223">
-        <v>221.625</v>
+        <v>621.625</v>
       </c>
       <c r="I223">
-        <v>22.162500000000001</v>
+        <v>62.162500000000001</v>
       </c>
       <c r="U223">
         <v>22.303138732910156</v>
@@ -10472,10 +10472,10 @@
         <v>61</v>
       </c>
       <c r="H224">
-        <v>221.125</v>
+        <v>621.125</v>
       </c>
       <c r="I224">
-        <v>22.112500000000001</v>
+        <v>62.112499999999997</v>
       </c>
       <c r="U224">
         <v>20.506156921386719</v>
@@ -10522,10 +10522,10 @@
         <v>61</v>
       </c>
       <c r="H225">
-        <v>388.75</v>
+        <v>788.75</v>
       </c>
       <c r="I225">
-        <v>38.875</v>
+        <v>78.875</v>
       </c>
       <c r="U225">
         <v>25.379058837890625</v>
@@ -10572,10 +10572,10 @@
         <v>61</v>
       </c>
       <c r="H226">
-        <v>845.125</v>
+        <v>1245.125</v>
       </c>
       <c r="I226">
-        <v>84.512500000000003</v>
+        <v>124.5125</v>
       </c>
       <c r="U226">
         <v>24.353496551513672</v>
@@ -10622,10 +10622,10 @@
         <v>61</v>
       </c>
       <c r="H227">
-        <v>290.25</v>
+        <v>690.25</v>
       </c>
       <c r="I227">
-        <v>29.024999999999999</v>
+        <v>69.025000000000006</v>
       </c>
       <c r="U227">
         <v>24.742202758789063</v>
@@ -10672,10 +10672,10 @@
         <v>62</v>
       </c>
       <c r="H228">
-        <v>439.25</v>
+        <v>839.25</v>
       </c>
       <c r="I228">
-        <v>43.924999999999997</v>
+        <v>83.924999999999997</v>
       </c>
       <c r="U228">
         <v>22.571266174316406</v>
@@ -10722,10 +10722,10 @@
         <v>62</v>
       </c>
       <c r="H229">
-        <v>478.75</v>
+        <v>878.75</v>
       </c>
       <c r="I229">
-        <v>47.875</v>
+        <v>87.875</v>
       </c>
       <c r="U229">
         <v>19.276674270629883</v>
@@ -10772,10 +10772,10 @@
         <v>62</v>
       </c>
       <c r="H230">
-        <v>566.375</v>
+        <v>966.375</v>
       </c>
       <c r="I230">
-        <v>56.637500000000003</v>
+        <v>96.637500000000003</v>
       </c>
       <c r="U230">
         <v>17.341087341308594</v>
@@ -10822,10 +10822,10 @@
         <v>62</v>
       </c>
       <c r="H231">
-        <v>576.125</v>
+        <v>976.125</v>
       </c>
       <c r="I231">
-        <v>57.612499999999997</v>
+        <v>97.612499999999997</v>
       </c>
       <c r="U231">
         <v>18.378559112548828</v>
@@ -10872,10 +10872,10 @@
         <v>62</v>
       </c>
       <c r="H232">
-        <v>379.625</v>
+        <v>779.625</v>
       </c>
       <c r="I232">
-        <v>37.962499999999999</v>
+        <v>77.962500000000006</v>
       </c>
       <c r="U232">
         <v>19.524559020996094</v>
@@ -10922,10 +10922,10 @@
         <v>62</v>
       </c>
       <c r="H233">
-        <v>545.25</v>
+        <v>945.25</v>
       </c>
       <c r="I233">
-        <v>54.524999999999999</v>
+        <v>94.525000000000006</v>
       </c>
       <c r="U233">
         <v>24.697391510009766</v>
@@ -10972,10 +10972,10 @@
         <v>62</v>
       </c>
       <c r="H234">
-        <v>876</v>
+        <v>1276</v>
       </c>
       <c r="I234">
-        <v>87.6</v>
+        <v>127.6</v>
       </c>
       <c r="U234">
         <v>18.123012542724609</v>
@@ -11022,10 +11022,10 @@
         <v>62</v>
       </c>
       <c r="H235">
-        <v>393</v>
+        <v>793</v>
       </c>
       <c r="I235">
-        <v>39.299999999999997</v>
+        <v>79.3</v>
       </c>
     </row>
     <row r="236" spans="1:28" x14ac:dyDescent="0.25">
@@ -11048,10 +11048,10 @@
         <v>62</v>
       </c>
       <c r="H236">
-        <v>528.125</v>
+        <v>928.125</v>
       </c>
       <c r="I236">
-        <v>52.8125</v>
+        <v>92.8125</v>
       </c>
       <c r="U236">
         <v>18.850322723388672</v>
@@ -11098,10 +11098,10 @@
         <v>62</v>
       </c>
       <c r="H237">
-        <v>505.37500000000011</v>
+        <v>905.37500000000011</v>
       </c>
       <c r="I237">
-        <v>50.537500000000009</v>
+        <v>90.537500000000009</v>
       </c>
       <c r="U237">
         <v>20.164098739624023</v>
@@ -11148,10 +11148,10 @@
         <v>62</v>
       </c>
       <c r="H238">
-        <v>674.875</v>
+        <v>1074.875</v>
       </c>
       <c r="I238">
-        <v>67.487499999999997</v>
+        <v>107.4875</v>
       </c>
       <c r="U238">
         <v>18.740419387817383</v>
@@ -11198,10 +11198,10 @@
         <v>62</v>
       </c>
       <c r="H239">
-        <v>251.75</v>
+        <v>651.75</v>
       </c>
       <c r="I239">
-        <v>25.175000000000001</v>
+        <v>65.174999999999997</v>
       </c>
       <c r="U239">
         <v>21.048513412475586</v>
@@ -11248,10 +11248,10 @@
         <v>62</v>
       </c>
       <c r="H240">
-        <v>596.625</v>
+        <v>996.625</v>
       </c>
       <c r="I240">
-        <v>59.662500000000001</v>
+        <v>99.662499999999994</v>
       </c>
       <c r="U240">
         <v>22.900033950805664</v>
@@ -11298,10 +11298,10 @@
         <v>62</v>
       </c>
       <c r="H241">
-        <v>285.25</v>
+        <v>685.25</v>
       </c>
       <c r="I241">
-        <v>28.524999999999999</v>
+        <v>68.525000000000006</v>
       </c>
       <c r="U241">
         <v>20.319797515869141</v>
@@ -11348,10 +11348,10 @@
         <v>62</v>
       </c>
       <c r="H242">
-        <v>471.375</v>
+        <v>871.375</v>
       </c>
       <c r="I242">
-        <v>47.137500000000003</v>
+        <v>87.137500000000003</v>
       </c>
       <c r="U242">
         <v>18.326526641845703</v>
@@ -11398,10 +11398,10 @@
         <v>62</v>
       </c>
       <c r="H243">
-        <v>391</v>
+        <v>791</v>
       </c>
       <c r="I243">
-        <v>39.1</v>
+        <v>79.099999999999994</v>
       </c>
       <c r="U243">
         <v>19.630317687988281</v>
@@ -11448,10 +11448,10 @@
         <v>62</v>
       </c>
       <c r="H244">
-        <v>618.5</v>
+        <v>1018.5</v>
       </c>
       <c r="I244">
-        <v>61.85</v>
+        <v>101.85</v>
       </c>
       <c r="U244">
         <v>17.620277404785156</v>
@@ -11498,10 +11498,10 @@
         <v>62</v>
       </c>
       <c r="H245">
-        <v>399.375</v>
+        <v>799.375</v>
       </c>
       <c r="I245">
-        <v>39.9375</v>
+        <v>79.9375</v>
       </c>
       <c r="U245">
         <v>21.181156158447266</v>
@@ -11548,10 +11548,10 @@
         <v>63</v>
       </c>
       <c r="H246">
-        <v>510.375</v>
+        <v>910.375</v>
       </c>
       <c r="I246">
-        <v>51.037500000000001</v>
+        <v>91.037499999999994</v>
       </c>
       <c r="U246">
         <v>21.888200759887695</v>
@@ -11598,10 +11598,10 @@
         <v>63</v>
       </c>
       <c r="H247">
-        <v>1040.75</v>
+        <v>1440.75</v>
       </c>
       <c r="I247">
-        <v>104.075</v>
+        <v>144.07499999999999</v>
       </c>
       <c r="U247">
         <v>19.746637344360352</v>
@@ -11648,10 +11648,10 @@
         <v>63</v>
       </c>
       <c r="H248">
-        <v>1268.625</v>
+        <v>1668.625</v>
       </c>
       <c r="I248">
-        <v>126.8625</v>
+        <v>166.86250000000001</v>
       </c>
       <c r="U248">
         <v>18.557491302490234</v>
@@ -11698,10 +11698,10 @@
         <v>63</v>
       </c>
       <c r="H249">
-        <v>1318</v>
+        <v>1718</v>
       </c>
       <c r="I249">
-        <v>131.80000000000001</v>
+        <v>171.8</v>
       </c>
       <c r="U249">
         <v>19.320089340209961</v>
@@ -11748,10 +11748,10 @@
         <v>63</v>
       </c>
       <c r="H250">
-        <v>365.625</v>
+        <v>765.625</v>
       </c>
       <c r="I250">
-        <v>36.5625</v>
+        <v>76.5625</v>
       </c>
       <c r="U250">
         <v>20.214420318603516</v>
@@ -11798,10 +11798,10 @@
         <v>63</v>
       </c>
       <c r="H251">
-        <v>530.625</v>
+        <v>930.625</v>
       </c>
       <c r="I251">
-        <v>53.0625</v>
+        <v>93.0625</v>
       </c>
       <c r="U251">
         <v>19.546619415283203</v>
@@ -11848,10 +11848,10 @@
         <v>63</v>
       </c>
       <c r="H252">
-        <v>1421.5</v>
+        <v>1821.5</v>
       </c>
       <c r="I252">
-        <v>142.15</v>
+        <v>182.15</v>
       </c>
       <c r="U252">
         <v>19.22789192199707</v>
@@ -11898,10 +11898,10 @@
         <v>63</v>
       </c>
       <c r="H253">
-        <v>1071.125</v>
+        <v>1471.125</v>
       </c>
       <c r="I253">
-        <v>107.1125</v>
+        <v>147.11250000000001</v>
       </c>
       <c r="U253">
         <v>19.012954711914062</v>
@@ -11948,10 +11948,10 @@
         <v>63</v>
       </c>
       <c r="H254">
-        <v>1608.625</v>
+        <v>2008.625</v>
       </c>
       <c r="I254">
-        <v>160.86250000000001</v>
+        <v>200.86250000000001</v>
       </c>
       <c r="U254">
         <v>19.394535064697266</v>
@@ -11998,10 +11998,10 @@
         <v>63</v>
       </c>
       <c r="H255">
-        <v>1464.125</v>
+        <v>1864.125</v>
       </c>
       <c r="I255">
-        <v>146.41249999999999</v>
+        <v>186.41249999999999</v>
       </c>
       <c r="U255">
         <v>19.320266723632813</v>
@@ -12048,10 +12048,10 @@
         <v>63</v>
       </c>
       <c r="H256">
-        <v>1379.625</v>
+        <v>1779.625</v>
       </c>
       <c r="I256">
-        <v>137.96250000000001</v>
+        <v>177.96250000000001</v>
       </c>
       <c r="U256">
         <v>19.770790100097656</v>
@@ -12098,10 +12098,10 @@
         <v>63</v>
       </c>
       <c r="H257">
-        <v>1126.125</v>
+        <v>1526.125</v>
       </c>
       <c r="I257">
-        <v>112.6125</v>
+        <v>152.61250000000001</v>
       </c>
       <c r="U257">
         <v>19.844314575195313</v>
@@ -12148,10 +12148,10 @@
         <v>63</v>
       </c>
       <c r="H258">
-        <v>1092</v>
+        <v>1492</v>
       </c>
       <c r="I258">
-        <v>109.2</v>
+        <v>149.19999999999999</v>
       </c>
       <c r="U258">
         <v>19.105487823486328</v>
@@ -12198,10 +12198,10 @@
         <v>63</v>
       </c>
       <c r="H259">
-        <v>980.5</v>
+        <v>1380.5</v>
       </c>
       <c r="I259">
-        <v>98.05</v>
+        <v>138.05000000000001</v>
       </c>
       <c r="U259">
         <v>19.353839874267578</v>
@@ -12248,10 +12248,10 @@
         <v>63</v>
       </c>
       <c r="H260">
-        <v>1163</v>
+        <v>1563</v>
       </c>
       <c r="I260">
-        <v>116.3</v>
+        <v>156.30000000000001</v>
       </c>
       <c r="U260">
         <v>19.39324951171875</v>
@@ -12298,10 +12298,10 @@
         <v>63</v>
       </c>
       <c r="H261">
-        <v>1302.125</v>
+        <v>1702.125</v>
       </c>
       <c r="I261">
-        <v>130.21250000000001</v>
+        <v>170.21250000000001</v>
       </c>
       <c r="U261">
         <v>20.463342666625977</v>
@@ -12348,10 +12348,10 @@
         <v>63</v>
       </c>
       <c r="H262">
-        <v>1785.25</v>
+        <v>2185.25</v>
       </c>
       <c r="I262">
-        <v>178.52500000000001</v>
+        <v>218.52500000000001</v>
       </c>
       <c r="U262">
         <v>16.442989349365234</v>
@@ -12398,10 +12398,10 @@
         <v>63</v>
       </c>
       <c r="H263">
-        <v>930.625</v>
+        <v>1330.625</v>
       </c>
       <c r="I263">
-        <v>93.0625</v>
+        <v>133.0625</v>
       </c>
       <c r="U263">
         <v>19.560453414916992</v>
@@ -17248,10 +17248,10 @@
         <v>61</v>
       </c>
       <c r="H360">
-        <v>136.125</v>
+        <v>536.125</v>
       </c>
       <c r="I360">
-        <v>13.612500000000001</v>
+        <v>53.612499999999997</v>
       </c>
       <c r="U360">
         <v>19.363189697265625</v>
@@ -17298,10 +17298,10 @@
         <v>61</v>
       </c>
       <c r="H361">
-        <v>151.875</v>
+        <v>551.875</v>
       </c>
       <c r="I361">
-        <v>15.1875</v>
+        <v>55.1875</v>
       </c>
       <c r="U361">
         <v>20.846580505371094</v>
@@ -17348,10 +17348,10 @@
         <v>61</v>
       </c>
       <c r="H362">
-        <v>275.5</v>
+        <v>675.5</v>
       </c>
       <c r="I362">
-        <v>27.55</v>
+        <v>67.55</v>
       </c>
       <c r="U362">
         <v>19.745090484619141</v>
@@ -17398,10 +17398,10 @@
         <v>61</v>
       </c>
       <c r="H363">
-        <v>236.125</v>
+        <v>636.125</v>
       </c>
       <c r="I363">
-        <v>23.612500000000001</v>
+        <v>63.612499999999997</v>
       </c>
       <c r="U363">
         <v>19.933826446533203</v>
@@ -17448,10 +17448,10 @@
         <v>61</v>
       </c>
       <c r="H364">
-        <v>79.375</v>
+        <v>479.375</v>
       </c>
       <c r="I364">
-        <v>7.9375</v>
+        <v>47.9375</v>
       </c>
       <c r="U364">
         <v>21.304208755493164</v>
@@ -17498,10 +17498,10 @@
         <v>61</v>
       </c>
       <c r="H365">
-        <v>295.625</v>
+        <v>695.625</v>
       </c>
       <c r="I365">
-        <v>29.5625</v>
+        <v>69.5625</v>
       </c>
       <c r="U365">
         <v>20.105375289916992</v>
@@ -17548,10 +17548,10 @@
         <v>61</v>
       </c>
       <c r="H366">
-        <v>301.375</v>
+        <v>701.375</v>
       </c>
       <c r="I366">
-        <v>30.137499999999999</v>
+        <v>70.137500000000003</v>
       </c>
       <c r="U366">
         <v>19.139392852783203</v>
@@ -17598,10 +17598,10 @@
         <v>61</v>
       </c>
       <c r="H367">
-        <v>159.625</v>
+        <v>559.625</v>
       </c>
       <c r="I367">
-        <v>15.9625</v>
+        <v>55.962499999999999</v>
       </c>
       <c r="U367">
         <v>20.868686676025391</v>
@@ -17648,10 +17648,10 @@
         <v>61</v>
       </c>
       <c r="H368">
-        <v>234.875</v>
+        <v>634.875</v>
       </c>
       <c r="I368">
-        <v>23.487500000000001</v>
+        <v>63.487499999999997</v>
       </c>
       <c r="U368">
         <v>19.552951812744141</v>
@@ -17698,10 +17698,10 @@
         <v>61</v>
       </c>
       <c r="H369">
-        <v>212.25</v>
+        <v>612.25</v>
       </c>
       <c r="I369">
-        <v>21.225000000000001</v>
+        <v>61.225000000000001</v>
       </c>
       <c r="U369">
         <v>21.454952239990234</v>
@@ -17748,10 +17748,10 @@
         <v>61</v>
       </c>
       <c r="H370">
-        <v>255.625</v>
+        <v>655.625</v>
       </c>
       <c r="I370">
-        <v>25.5625</v>
+        <v>65.5625</v>
       </c>
       <c r="U370">
         <v>20.894657135009766</v>
@@ -17798,10 +17798,10 @@
         <v>61</v>
       </c>
       <c r="H371">
-        <v>133.125</v>
+        <v>533.125</v>
       </c>
       <c r="I371">
-        <v>13.3125</v>
+        <v>53.3125</v>
       </c>
       <c r="U371">
         <v>20.72991943359375</v>
@@ -17848,10 +17848,10 @@
         <v>61</v>
       </c>
       <c r="H372">
-        <v>426.875</v>
+        <v>826.875</v>
       </c>
       <c r="I372">
-        <v>42.6875</v>
+        <v>82.6875</v>
       </c>
       <c r="U372">
         <v>21.550785064697266</v>
@@ -17898,10 +17898,10 @@
         <v>61</v>
       </c>
       <c r="H373">
-        <v>231.625</v>
+        <v>631.625</v>
       </c>
       <c r="I373">
-        <v>23.162500000000001</v>
+        <v>63.162500000000001</v>
       </c>
       <c r="U373">
         <v>22.251811981201172</v>
@@ -17948,10 +17948,10 @@
         <v>61</v>
       </c>
       <c r="H374">
-        <v>348.625</v>
+        <v>748.625</v>
       </c>
       <c r="I374">
-        <v>34.862499999999997</v>
+        <v>74.862499999999997</v>
       </c>
       <c r="U374">
         <v>22.155685424804688</v>
@@ -17998,10 +17998,10 @@
         <v>61</v>
       </c>
       <c r="H375">
-        <v>64.125</v>
+        <v>464.125</v>
       </c>
       <c r="I375">
-        <v>6.4124999999999996</v>
+        <v>46.412500000000001</v>
       </c>
       <c r="U375">
         <v>20.149831771850586</v>
@@ -18048,10 +18048,10 @@
         <v>61</v>
       </c>
       <c r="H376">
-        <v>276.5</v>
+        <v>676.5</v>
       </c>
       <c r="I376">
-        <v>27.65</v>
+        <v>67.650000000000006</v>
       </c>
       <c r="U376">
         <v>19.663623809814453</v>
@@ -18098,10 +18098,10 @@
         <v>61</v>
       </c>
       <c r="H377">
-        <v>120.625</v>
+        <v>520.625</v>
       </c>
       <c r="I377">
-        <v>12.0625</v>
+        <v>52.0625</v>
       </c>
       <c r="U377">
         <v>20.352630615234375</v>
@@ -18148,10 +18148,10 @@
         <v>62</v>
       </c>
       <c r="H378">
-        <v>1007.4999999999999</v>
+        <v>1407.5</v>
       </c>
       <c r="I378">
-        <v>100.74999999999999</v>
+        <v>140.75</v>
       </c>
       <c r="U378">
         <v>21.028469085693359</v>
@@ -18198,10 +18198,10 @@
         <v>62</v>
       </c>
       <c r="H379">
-        <v>533.875</v>
+        <v>933.875</v>
       </c>
       <c r="I379">
-        <v>53.387500000000003</v>
+        <v>93.387500000000003</v>
       </c>
       <c r="U379">
         <v>20.905948638916016</v>
@@ -18248,10 +18248,10 @@
         <v>62</v>
       </c>
       <c r="H380">
-        <v>2103.375</v>
+        <v>2503.375</v>
       </c>
       <c r="I380">
-        <v>210.33750000000001</v>
+        <v>250.33750000000001</v>
       </c>
       <c r="U380">
         <v>21.376592636108398</v>
@@ -18298,10 +18298,10 @@
         <v>62</v>
       </c>
       <c r="H381">
-        <v>1514.5</v>
+        <v>1914.5</v>
       </c>
       <c r="I381">
-        <v>151.44999999999999</v>
+        <v>191.45</v>
       </c>
       <c r="U381">
         <v>18.526302337646484</v>
@@ -18348,10 +18348,10 @@
         <v>62</v>
       </c>
       <c r="H382">
-        <v>963.25</v>
+        <v>1363.25</v>
       </c>
       <c r="I382">
-        <v>96.325000000000003</v>
+        <v>136.32499999999999</v>
       </c>
       <c r="U382">
         <v>22.064830780029297</v>
@@ -18398,10 +18398,10 @@
         <v>62</v>
       </c>
       <c r="H383">
-        <v>999.625</v>
+        <v>1399.625</v>
       </c>
       <c r="I383">
-        <v>99.962500000000006</v>
+        <v>139.96250000000001</v>
       </c>
       <c r="U383">
         <v>22.527065277099609</v>
@@ -18448,10 +18448,10 @@
         <v>62</v>
       </c>
       <c r="H384">
-        <v>1917</v>
+        <v>2317</v>
       </c>
       <c r="I384">
-        <v>191.7</v>
+        <v>231.7</v>
       </c>
       <c r="U384">
         <v>17.93621826171875</v>
@@ -18498,10 +18498,10 @@
         <v>62</v>
       </c>
       <c r="H385">
-        <v>843.875</v>
+        <v>1243.875</v>
       </c>
       <c r="I385">
-        <v>84.387500000000003</v>
+        <v>124.3875</v>
       </c>
       <c r="U385">
         <v>21.747386932373047</v>
@@ -18548,10 +18548,10 @@
         <v>62</v>
       </c>
       <c r="H386">
-        <v>1446</v>
+        <v>1846</v>
       </c>
       <c r="I386">
-        <v>144.6</v>
+        <v>184.6</v>
       </c>
       <c r="U386">
         <v>19.365476608276367</v>
@@ -18598,10 +18598,10 @@
         <v>62</v>
       </c>
       <c r="H387">
-        <v>1022.375</v>
+        <v>1422.375</v>
       </c>
       <c r="I387">
-        <v>102.2375</v>
+        <v>142.23750000000001</v>
       </c>
       <c r="U387">
         <v>20.797229766845703</v>
@@ -18648,10 +18648,10 @@
         <v>62</v>
       </c>
       <c r="H388">
-        <v>1583.25</v>
+        <v>1983.25</v>
       </c>
       <c r="I388">
-        <v>158.32499999999999</v>
+        <v>198.32499999999999</v>
       </c>
       <c r="U388">
         <v>20.983640670776367</v>
@@ -18698,10 +18698,10 @@
         <v>62</v>
       </c>
       <c r="H389">
-        <v>981</v>
+        <v>1381</v>
       </c>
       <c r="I389">
-        <v>98.1</v>
+        <v>138.1</v>
       </c>
       <c r="U389">
         <v>21.501506805419922</v>
@@ -18748,10 +18748,10 @@
         <v>62</v>
       </c>
       <c r="H390">
-        <v>903.5</v>
+        <v>1303.5</v>
       </c>
       <c r="I390">
-        <v>90.35</v>
+        <v>130.35</v>
       </c>
       <c r="U390">
         <v>21.703550338745117</v>
@@ -18798,10 +18798,10 @@
         <v>62</v>
       </c>
       <c r="H391">
-        <v>663.75</v>
+        <v>1063.75</v>
       </c>
       <c r="I391">
-        <v>66.375</v>
+        <v>106.375</v>
       </c>
       <c r="U391">
         <v>22.45013427734375</v>
@@ -18848,10 +18848,10 @@
         <v>62</v>
       </c>
       <c r="H392">
-        <v>1569.25</v>
+        <v>1969.25</v>
       </c>
       <c r="I392">
-        <v>156.92500000000001</v>
+        <v>196.92500000000001</v>
       </c>
       <c r="U392">
         <v>22.191417694091797</v>
@@ -18898,10 +18898,10 @@
         <v>62</v>
       </c>
       <c r="H393">
-        <v>1236.875</v>
+        <v>1636.875</v>
       </c>
       <c r="I393">
-        <v>123.6875</v>
+        <v>163.6875</v>
       </c>
       <c r="U393">
         <v>21.588232040405273</v>
@@ -18948,10 +18948,10 @@
         <v>62</v>
       </c>
       <c r="H394">
-        <v>1742.125</v>
+        <v>2142.125</v>
       </c>
       <c r="I394">
-        <v>174.21250000000001</v>
+        <v>214.21250000000001</v>
       </c>
       <c r="U394">
         <v>18.798074722290039</v>
@@ -18998,10 +18998,10 @@
         <v>62</v>
       </c>
       <c r="H395">
-        <v>1307.125</v>
+        <v>1707.125</v>
       </c>
       <c r="I395">
-        <v>130.71250000000001</v>
+        <v>170.71250000000001</v>
       </c>
       <c r="U395">
         <v>20.794073104858398</v>
@@ -24682,10 +24682,10 @@
         <v>85</v>
       </c>
       <c r="H516">
-        <v>523.75</v>
+        <v>923.75</v>
       </c>
       <c r="I516">
-        <v>52.375</v>
+        <v>92.375</v>
       </c>
       <c r="U516">
         <v>23.346094131469727</v>
@@ -24729,10 +24729,10 @@
         <v>85</v>
       </c>
       <c r="H517">
-        <v>900.75</v>
+        <v>1300.75</v>
       </c>
       <c r="I517">
-        <v>90.075000000000003</v>
+        <v>130.07499999999999</v>
       </c>
       <c r="U517">
         <v>19.541614532470703</v>
@@ -24776,10 +24776,10 @@
         <v>85</v>
       </c>
       <c r="H518">
-        <v>1044.75</v>
+        <v>1444.75</v>
       </c>
       <c r="I518">
-        <v>104.47499999999999</v>
+        <v>144.47499999999999</v>
       </c>
       <c r="U518">
         <v>16.759342193603516</v>
@@ -24823,10 +24823,10 @@
         <v>85</v>
       </c>
       <c r="H519">
-        <v>1041</v>
+        <v>1441</v>
       </c>
       <c r="I519">
-        <v>104.1</v>
+        <v>144.1</v>
       </c>
       <c r="U519">
         <v>19.566349029541016</v>
@@ -24870,10 +24870,10 @@
         <v>85</v>
       </c>
       <c r="H520">
-        <v>394.75</v>
+        <v>794.75</v>
       </c>
       <c r="I520">
-        <v>39.475000000000001</v>
+        <v>79.474999999999994</v>
       </c>
       <c r="U520">
         <v>20.142532348632812</v>
@@ -24917,10 +24917,10 @@
         <v>85</v>
       </c>
       <c r="H521">
-        <v>451.875</v>
+        <v>851.875</v>
       </c>
       <c r="I521">
-        <v>45.1875</v>
+        <v>85.1875</v>
       </c>
       <c r="U521">
         <v>19.89710807800293</v>
@@ -24964,10 +24964,10 @@
         <v>85</v>
       </c>
       <c r="H522">
-        <v>1146</v>
+        <v>1546</v>
       </c>
       <c r="I522">
-        <v>114.6</v>
+        <v>154.6</v>
       </c>
       <c r="U522">
         <v>17.206214904785156</v>
@@ -25011,10 +25011,10 @@
         <v>85</v>
       </c>
       <c r="H523">
-        <v>710</v>
+        <v>1110</v>
       </c>
       <c r="I523">
-        <v>71</v>
+        <v>111</v>
       </c>
     </row>
     <row r="524" spans="1:28" x14ac:dyDescent="0.25">
@@ -25034,10 +25034,10 @@
         <v>85</v>
       </c>
       <c r="H524">
-        <v>1043.75</v>
+        <v>1443.75</v>
       </c>
       <c r="I524">
-        <v>104.375</v>
+        <v>144.375</v>
       </c>
       <c r="U524">
         <v>19.390880584716797</v>
@@ -25081,10 +25081,10 @@
         <v>85</v>
       </c>
       <c r="H525">
-        <v>680.5</v>
+        <v>1080.5</v>
       </c>
       <c r="I525">
-        <v>68.05</v>
+        <v>108.05</v>
       </c>
       <c r="U525">
         <v>19.467626571655273</v>
@@ -25128,10 +25128,10 @@
         <v>85</v>
       </c>
       <c r="H526">
-        <v>911.5</v>
+        <v>1311.5</v>
       </c>
       <c r="I526">
-        <v>91.15</v>
+        <v>131.15</v>
       </c>
       <c r="U526">
         <v>19.182683944702148</v>
@@ -25175,10 +25175,10 @@
         <v>85</v>
       </c>
       <c r="H527">
-        <v>473.375</v>
+        <v>873.375</v>
       </c>
       <c r="I527">
-        <v>47.337499999999999</v>
+        <v>87.337500000000006</v>
       </c>
       <c r="U527">
         <v>20.558544158935547</v>
@@ -25222,10 +25222,10 @@
         <v>85</v>
       </c>
       <c r="H528">
-        <v>666</v>
+        <v>1066</v>
       </c>
       <c r="I528">
-        <v>66.599999999999994</v>
+        <v>106.6</v>
       </c>
       <c r="U528">
         <v>19.539247512817383</v>
@@ -25269,10 +25269,10 @@
         <v>85</v>
       </c>
       <c r="H529">
-        <v>735.25</v>
+        <v>1135.25</v>
       </c>
       <c r="I529">
-        <v>73.525000000000006</v>
+        <v>113.52500000000001</v>
       </c>
       <c r="U529">
         <v>20.711856842041016</v>
@@ -25316,10 +25316,10 @@
         <v>85</v>
       </c>
       <c r="H530">
-        <v>879.5</v>
+        <v>1279.5</v>
       </c>
       <c r="I530">
-        <v>87.95</v>
+        <v>127.95</v>
       </c>
       <c r="U530">
         <v>20.207330703735352</v>
@@ -25363,10 +25363,10 @@
         <v>85</v>
       </c>
       <c r="H531">
-        <v>800.125</v>
+        <v>1200.125</v>
       </c>
       <c r="I531">
-        <v>80.012500000000003</v>
+        <v>120.0125</v>
       </c>
       <c r="U531">
         <v>20.545780181884766</v>
@@ -25410,10 +25410,10 @@
         <v>85</v>
       </c>
       <c r="H532">
-        <v>1361.375</v>
+        <v>1761.375</v>
       </c>
       <c r="I532">
-        <v>136.13749999999999</v>
+        <v>176.13749999999999</v>
       </c>
       <c r="U532">
         <v>16.931575775146484</v>
@@ -25457,10 +25457,10 @@
         <v>85</v>
       </c>
       <c r="H533">
-        <v>402</v>
+        <v>802</v>
       </c>
       <c r="I533">
-        <v>40.200000000000003</v>
+        <v>80.2</v>
       </c>
       <c r="U533">
         <v>20.584064483642578</v>

</xml_diff>

<commit_message>
updating plantain model + delete incomplete test
</commit_message>
<xml_diff>
--- a/Prototypes/Plantain/Observed.xlsx
+++ b/Prototypes/Plantain/Observed.xlsx
@@ -309,16 +309,16 @@
     <t>Eval</t>
   </si>
   <si>
-    <t>RELARC_02CultivarsLancelot</t>
-  </si>
-  <si>
-    <t>RELARC_02CultivarsTonic</t>
-  </si>
-  <si>
     <t>No1FarmFD902GrazeFrequency2wks</t>
   </si>
   <si>
     <t>No1FarmFD902GrazeFrequency4wks</t>
+  </si>
+  <si>
+    <t>RELARC_02CultivarLancelot</t>
+  </si>
+  <si>
+    <t>RELARC_02CultivarTonic</t>
   </si>
 </sst>
 </file>
@@ -845,10 +845,10 @@
   <dimension ref="A1:AI1519"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F209" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K209" sqref="K209"/>
+      <selection pane="bottomRight" activeCell="J2" sqref="J2:J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,7 +1001,7 @@
         <v>45</v>
       </c>
       <c r="J2">
-        <v>160.1</v>
+        <v>143.9</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
@@ -1018,7 +1018,7 @@
         <v>45</v>
       </c>
       <c r="J3">
-        <v>115.6</v>
+        <v>143.9</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
@@ -1035,7 +1035,7 @@
         <v>45</v>
       </c>
       <c r="J4">
-        <v>160.1</v>
+        <v>143.9</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
@@ -1052,7 +1052,7 @@
         <v>45</v>
       </c>
       <c r="J5">
-        <v>115.6</v>
+        <v>143.9</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
@@ -1069,7 +1069,7 @@
         <v>45</v>
       </c>
       <c r="J6">
-        <v>73.7</v>
+        <v>66.2</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
@@ -1086,7 +1086,7 @@
         <v>45</v>
       </c>
       <c r="J7">
-        <v>42.6</v>
+        <v>38.299999999999997</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
@@ -1103,7 +1103,7 @@
         <v>45</v>
       </c>
       <c r="J8">
-        <v>35</v>
+        <v>22.8</v>
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
@@ -1120,7 +1120,7 @@
         <v>45</v>
       </c>
       <c r="J9">
-        <v>257.7</v>
+        <v>226.9</v>
       </c>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.25">
@@ -1137,7 +1137,7 @@
         <v>45</v>
       </c>
       <c r="J10">
-        <v>257.7</v>
+        <v>226.9</v>
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
@@ -1154,7 +1154,7 @@
         <v>45</v>
       </c>
       <c r="J11">
-        <v>148.1</v>
+        <v>257.5</v>
       </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.25">
@@ -1171,7 +1171,7 @@
         <v>45</v>
       </c>
       <c r="J12">
-        <v>63.9</v>
+        <v>56.2</v>
       </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
@@ -1188,7 +1188,7 @@
         <v>45</v>
       </c>
       <c r="J13">
-        <v>69.8</v>
+        <v>29.6</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
@@ -1205,7 +1205,7 @@
         <v>45</v>
       </c>
       <c r="J14">
-        <v>149.4</v>
+        <v>134.30000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
@@ -1222,7 +1222,7 @@
         <v>45</v>
       </c>
       <c r="J15">
-        <v>107.9</v>
+        <v>134.30000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
@@ -1239,7 +1239,7 @@
         <v>45</v>
       </c>
       <c r="J16">
-        <v>149.4</v>
+        <v>134.30000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -1256,7 +1256,7 @@
         <v>45</v>
       </c>
       <c r="J17">
-        <v>107.9</v>
+        <v>134.30000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -1273,7 +1273,7 @@
         <v>45</v>
       </c>
       <c r="J18">
-        <v>68.8</v>
+        <v>61.8</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -1290,7 +1290,7 @@
         <v>45</v>
       </c>
       <c r="J19">
-        <v>39.799999999999997</v>
+        <v>35.700000000000003</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1307,7 +1307,7 @@
         <v>45</v>
       </c>
       <c r="J20">
-        <v>32.700000000000003</v>
+        <v>21.3</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -1324,7 +1324,7 @@
         <v>45</v>
       </c>
       <c r="J21">
-        <v>240.5</v>
+        <v>211.8</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -1341,7 +1341,7 @@
         <v>45</v>
       </c>
       <c r="J22">
-        <v>240.5</v>
+        <v>211.8</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -1358,7 +1358,7 @@
         <v>45</v>
       </c>
       <c r="J23">
-        <v>138.19999999999999</v>
+        <v>240.4</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -1375,7 +1375,7 @@
         <v>45</v>
       </c>
       <c r="J24">
-        <v>59.6</v>
+        <v>52.5</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -1392,12 +1392,12 @@
         <v>45</v>
       </c>
       <c r="J25">
-        <v>65.099999999999994</v>
+        <v>27.7</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B26" t="s">
         <v>92</v>
@@ -1414,7 +1414,7 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B27" t="s">
         <v>92</v>
@@ -1426,12 +1426,12 @@
         <v>45</v>
       </c>
       <c r="J27">
-        <v>183.5</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B28" t="s">
         <v>92</v>
@@ -1443,12 +1443,12 @@
         <v>45</v>
       </c>
       <c r="J28">
-        <v>156.9</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B29" t="s">
         <v>92</v>
@@ -1460,12 +1460,12 @@
         <v>45</v>
       </c>
       <c r="J29">
-        <v>112.5</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B30" t="s">
         <v>92</v>
@@ -1477,12 +1477,12 @@
         <v>45</v>
       </c>
       <c r="J30">
-        <v>64.400000000000006</v>
+        <v>62.4</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B31" t="s">
         <v>92</v>
@@ -1494,12 +1494,12 @@
         <v>45</v>
       </c>
       <c r="J31">
-        <v>32.700000000000003</v>
+        <v>31.7</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B32" t="s">
         <v>92</v>
@@ -1516,7 +1516,7 @@
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B33" t="s">
         <v>92</v>
@@ -1533,7 +1533,7 @@
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B34" t="s">
         <v>92</v>
@@ -1550,7 +1550,7 @@
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B35" t="s">
         <v>92</v>
@@ -1562,12 +1562,12 @@
         <v>45</v>
       </c>
       <c r="J35">
-        <v>166.8</v>
+        <v>138.19999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B36" t="s">
         <v>92</v>
@@ -1579,12 +1579,12 @@
         <v>45</v>
       </c>
       <c r="J36">
-        <v>142.69999999999999</v>
+        <v>138.19999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B37" t="s">
         <v>92</v>
@@ -1596,12 +1596,12 @@
         <v>45</v>
       </c>
       <c r="J37">
-        <v>102.2</v>
+        <v>138.19999999999999</v>
       </c>
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B38" t="s">
         <v>92</v>
@@ -1613,12 +1613,12 @@
         <v>45</v>
       </c>
       <c r="J38">
-        <v>58.6</v>
+        <v>56.7</v>
       </c>
     </row>
     <row r="39" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B39" t="s">
         <v>92</v>
@@ -1630,12 +1630,12 @@
         <v>45</v>
       </c>
       <c r="J39">
-        <v>29.7</v>
+        <v>28.8</v>
       </c>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B40" t="s">
         <v>92</v>
@@ -1652,7 +1652,7 @@
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B41" t="s">
         <v>92</v>
@@ -55675,7 +55675,7 @@
     </row>
     <row r="1488" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1488" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B1488" t="s">
         <v>55</v>
@@ -55698,7 +55698,7 @@
     </row>
     <row r="1489" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1489" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B1489" t="s">
         <v>55</v>
@@ -55718,7 +55718,7 @@
     </row>
     <row r="1490" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1490" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B1490" t="s">
         <v>55</v>
@@ -55741,7 +55741,7 @@
     </row>
     <row r="1491" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1491" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B1491" t="s">
         <v>55</v>
@@ -55761,7 +55761,7 @@
     </row>
     <row r="1492" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1492" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B1492" t="s">
         <v>55</v>
@@ -55784,7 +55784,7 @@
     </row>
     <row r="1493" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1493" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B1493" t="s">
         <v>55</v>
@@ -55804,7 +55804,7 @@
     </row>
     <row r="1494" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1494" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B1494" t="s">
         <v>55</v>
@@ -55827,7 +55827,7 @@
     </row>
     <row r="1495" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1495" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B1495" t="s">
         <v>55</v>
@@ -55847,7 +55847,7 @@
     </row>
     <row r="1496" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1496" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B1496" t="s">
         <v>55</v>
@@ -55870,7 +55870,7 @@
     </row>
     <row r="1497" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1497" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B1497" t="s">
         <v>55</v>
@@ -55890,7 +55890,7 @@
     </row>
     <row r="1498" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1498" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B1498" t="s">
         <v>55</v>
@@ -55913,7 +55913,7 @@
     </row>
     <row r="1499" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1499" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B1499" t="s">
         <v>55</v>
@@ -55933,7 +55933,7 @@
     </row>
     <row r="1500" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1500" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B1500" t="s">
         <v>55</v>
@@ -55956,7 +55956,7 @@
     </row>
     <row r="1501" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1501" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B1501" t="s">
         <v>55</v>
@@ -55976,7 +55976,7 @@
     </row>
     <row r="1502" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1502" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B1502" t="s">
         <v>55</v>
@@ -55999,7 +55999,7 @@
     </row>
     <row r="1503" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1503" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B1503" t="s">
         <v>55</v>
@@ -56019,7 +56019,7 @@
     </row>
     <row r="1504" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1504" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B1504" t="s">
         <v>55</v>
@@ -56042,7 +56042,7 @@
     </row>
     <row r="1505" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1505" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B1505" t="s">
         <v>55</v>
@@ -56062,7 +56062,7 @@
     </row>
     <row r="1506" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1506" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B1506" t="s">
         <v>55</v>
@@ -56085,7 +56085,7 @@
     </row>
     <row r="1507" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1507" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B1507" t="s">
         <v>55</v>
@@ -56105,7 +56105,7 @@
     </row>
     <row r="1508" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1508" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B1508" t="s">
         <v>55</v>
@@ -56128,7 +56128,7 @@
     </row>
     <row r="1509" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1509" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B1509" t="s">
         <v>55</v>
@@ -56148,7 +56148,7 @@
     </row>
     <row r="1510" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1510" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B1510" t="s">
         <v>55</v>
@@ -56171,7 +56171,7 @@
     </row>
     <row r="1511" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1511" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B1511" t="s">
         <v>55</v>
@@ -56191,7 +56191,7 @@
     </row>
     <row r="1512" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1512" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B1512" t="s">
         <v>55</v>
@@ -56214,7 +56214,7 @@
     </row>
     <row r="1513" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1513" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B1513" t="s">
         <v>55</v>
@@ -56234,7 +56234,7 @@
     </row>
     <row r="1514" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1514" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B1514" t="s">
         <v>55</v>
@@ -56257,7 +56257,7 @@
     </row>
     <row r="1515" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1515" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B1515" t="s">
         <v>55</v>
@@ -56277,7 +56277,7 @@
     </row>
     <row r="1516" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1516" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B1516" t="s">
         <v>55</v>
@@ -56300,7 +56300,7 @@
     </row>
     <row r="1517" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1517" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B1517" t="s">
         <v>55</v>
@@ -56320,7 +56320,7 @@
     </row>
     <row r="1518" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1518" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B1518" t="s">
         <v>55</v>
@@ -56343,7 +56343,7 @@
     </row>
     <row r="1519" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1519" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B1519" t="s">
         <v>55</v>

</xml_diff>